<commit_message>
prompt text updated, embeddings created
</commit_message>
<xml_diff>
--- a/data/describe/WVS_qualities.xlsx
+++ b/data/describe/WVS_qualities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy\Desktop\Green_Git\twelve-gpt-educational\data\describe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8BE1B5-EEA0-4745-968C-6CC128CF21D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEE4489-CE18-4FE4-A49D-B63862D5743B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t xml:space="preserve"> What are the two major dimensions of cultural variation identified by Inglehart and Welzel in the WVS?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The two dimensions are "Traditional values versus Secular-rational values" and "Survival values versus Self-expression values."</t>
   </si>
   <si>
     <t xml:space="preserve"> What do traditional values emphasize according to the WVS?</t>
@@ -70,25 +67,7 @@
     <t xml:space="preserve"> What are examples of questions related to Religiosity in the WVS?</t>
   </si>
   <si>
-    <t xml:space="preserve"> Questions include views on divorce, homosexuality, abortion, belief in the infallibility of religion, and the role of religious leaders in government.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Neutrality measures a lack of engagement in civic, political, or social organizations, with high-scoring countries having little participation in such groups.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Fairness is measured by attitudes toward whether actions like stealing, bribery, and violence are ever justifiable, reflecting societal values around justice.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> What does a high score in "Fairness" indicate?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> A high score indicates that a majority of the population believes actions like stealing and bribery are never justifiable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Scepticism represents distrust in large organizations and institutions, holding them accountable through democratic processes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> A high score indicates that a significant portion of the population has low confidence in major institutions such as government and corporations.</t>
   </si>
   <si>
     <t xml:space="preserve"> What does "Societal Tranquillity" measure?</t>
@@ -100,22 +79,10 @@
     <t xml:space="preserve"> What factors influence a low score in Societal Tranquillity?</t>
   </si>
   <si>
-    <t xml:space="preserve"> Low scores are influenced by high levels of societal anxiety about issues like war, terrorism, and economic stability.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> This dimension measures whether a society is focused on future rewards (Long-Term) or values traditions and short-term results (Short-Term).</t>
-  </si>
-  <si>
     <t xml:space="preserve"> What characterizes a society with Long-Term Orientation?</t>
   </si>
   <si>
-    <t xml:space="preserve"> Societies with Long-Term Orientation emphasize persistence, adaptability, and future rewards, with less focus on leisure.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> What is emphasized in Short-Term Orientation societies?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Short-Term Orientation societies prioritize quick results, social stability, and clear moral absolutes about good and evil.</t>
   </si>
   <si>
     <t xml:space="preserve"> How is "Religiosity" defined in the context of the WVS?</t>
@@ -140,6 +107,39 @@
   </si>
   <si>
     <t>assistant</t>
+  </si>
+  <si>
+    <t>The two major dimensions of cultural variation identified by Inglehart and Welzel in the WVS are "Traditional values versus Secular-rational values" and "Survival values versus Self-expression values."</t>
+  </si>
+  <si>
+    <t>Examples of questions related to religiosity include views on divorce, homosexuality, abortion, belief in the infallibility of religion, and the role of religious leaders in government.</t>
+  </si>
+  <si>
+    <t>Neutrality measures a lack of engagement in civic, political, or social organizations, with high-scoring countries having little participation in such groups.</t>
+  </si>
+  <si>
+    <t>Fairness is measured by attitudes toward whether actions like stealing, bribery, and violence are ever justifiable, reflecting societal values around justice.</t>
+  </si>
+  <si>
+    <t>Scepticism represents distrust in large organizations and institutions, holding them accountable through democratic processes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A high score in fairness indicates that a majority of the population believes actions like stealing and bribery are never justifiable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A high score in scepticism indicates that a significant portion of the population has low confidence in major institutions such as government and corporations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Low scores in tranquillity are influenced by high levels of societal anxiety about issues like war, terrorism, and economic stability.</t>
+  </si>
+  <si>
+    <t>The "Long- versus Short-Term Orientation" dimension measures whether a society is focused on future rewards (Long-Term) or values traditions and short-term results (Short-Term).</t>
+  </si>
+  <si>
+    <t>Societies with Long-Term Orientation emphasize persistence, adaptability, and future rewards, with less focus on leisure.</t>
+  </si>
+  <si>
+    <t>Short-Term Orientation societies prioritize quick results, social stability, and clear moral absolutes about good and evil.</t>
   </si>
 </sst>
 </file>
@@ -1374,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B941"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="59.08203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1386,10 +1386,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
@@ -1408,140 +1408,140 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="7" t="s">
+    </row>
+    <row r="6" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="7" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="7" t="s">
+    </row>
+    <row r="9" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+    <row r="10" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+    </row>
+    <row r="13" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B13" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="7" t="s">
+    <row r="17" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
+      <c r="B17" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B19" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="B20" s="7" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>